<commit_message>
Refactor from robot 2018 to VS Code.
</commit_message>
<xml_diff>
--- a/hardwareList.xlsx
+++ b/hardwareList.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fenix\workspace\robot2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Git\robot2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908BADF5-063D-419A-8AD3-59103CEED791}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
-    <sheet name="2019robot" sheetId="2" r:id="rId1"/>
-    <sheet name="2018robot" sheetId="1" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -286,7 +284,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,7 +481,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -778,36 +776,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001C930D-130E-4535-9998-E95F5C139305}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -830,7 +816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -850,7 +836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -867,7 +853,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -884,7 +870,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -901,7 +887,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -915,7 +901,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>13</v>
       </c>
@@ -923,7 +909,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -940,7 +926,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -960,7 +946,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>16</v>
@@ -978,14 +964,14 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="F13" s="2"/>
       <c r="L13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1005,7 +991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>16</v>
@@ -1020,7 +1006,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F16" s="2" t="s">
         <v>47</v>
       </c>
@@ -1028,7 +1014,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1045,7 +1031,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1059,7 +1045,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1073,7 +1059,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>35</v>
       </c>
@@ -1087,7 +1073,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
         <v>57</v>
       </c>
@@ -1098,7 +1084,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>84</v>
       </c>
@@ -1118,7 +1104,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>33</v>
       </c>
@@ -1132,7 +1118,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>33</v>
       </c>
@@ -1146,7 +1132,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>33</v>
       </c>
@@ -1160,7 +1146,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>33</v>
       </c>
@@ -1171,12 +1157,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1190,7 +1176,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>38</v>
       </c>
@@ -1201,7 +1187,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>65</v>
       </c>
@@ -1209,7 +1195,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -1220,7 +1206,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
         <v>68</v>
       </c>
@@ -1231,7 +1217,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
         <v>71</v>
       </c>
@@ -1239,7 +1225,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
         <v>73</v>
       </c>
@@ -1247,7 +1233,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>75</v>
       </c>
@@ -1255,7 +1241,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F42" s="3" t="s">
         <v>78</v>
       </c>

</xml_diff>